<commit_message>
Résolution de bugs + ajout du scraping du BNA
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmation\webscrapingproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA68647-F019-41BB-9B40-3323A0A059CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA254259-4DDA-4928-A148-42509E3256B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="592">
   <si>
     <t>CRIT</t>
   </si>
@@ -747,9 +747,6 @@
     <t>https://markets.ft.com/data/equities/tearsheet/summary?s=ATE:PAR</t>
   </si>
   <si>
-    <t>https://markets.ft.com/data/equities/tearsheet/summary?s=ALT:PAR</t>
-  </si>
-  <si>
     <t>http://www.zonebourse.com/ATOS-SE-4612/fondamentaux/</t>
   </si>
   <si>
@@ -807,9 +804,6 @@
     <t>https://markets.ft.com/data/equities/tearsheet/summary?s=BN:PAR</t>
   </si>
   <si>
-    <t>https://markets.ft.com/data/equities/tearsheet/summary?s=FLE:PAR</t>
-  </si>
-  <si>
     <t>https://markets.ft.com/data/equities/tearsheet/summary?s=CNP:PAR</t>
   </si>
   <si>
@@ -855,15 +849,9 @@
     <t>http://www.zonebourse.com/SCOR-SE-40096/fondamentaux/</t>
   </si>
   <si>
-    <t>https://markets.ft.com/data/equities/tearsheet/summary?s=BELI:PAR</t>
-  </si>
-  <si>
     <t>https://markets.ft.com/data/equities/tearsheet/summary?s=EO:PAR</t>
   </si>
   <si>
-    <t>https://markets.ft.com/data/equities/tearsheet/summary?s=MGIC:PAR</t>
-  </si>
-  <si>
     <t>https://markets.ft.com/data/equities/tearsheet/summary?s=ML:PAR</t>
   </si>
   <si>
@@ -1131,9 +1119,6 @@
     <t>http://www.zonebourse.com/ALBIOMA-5708/fondamentaux/</t>
   </si>
   <si>
-    <t>https://markets.ft.com/data/equities/tearsheet/summary?s=DIREN:PAR</t>
-  </si>
-  <si>
     <t>https://markets.ft.com/data/equities/tearsheet/summary?s=EDF:PAR</t>
   </si>
   <si>
@@ -1338,9 +1323,6 @@
     <t>http://www.zonebourse.com/VIVENDI-4727/fondamentaux/</t>
   </si>
   <si>
-    <t>https://markets.ft.com/data/equities/tearsheet/summary?s=GBB:PAR</t>
-  </si>
-  <si>
     <t>https://markets.ft.com/data/equities/tearsheet/summary?s=CGG:PAR</t>
   </si>
   <si>
@@ -1647,9 +1629,6 @@
     <t>http://www.zonebourse.com/ILIAD-4765/fondamentaux/</t>
   </si>
   <si>
-    <t>https://markets.ft.com/data/equities/tearsheet/summary?s=ATC:AEX</t>
-  </si>
-  <si>
     <t>https://markets.ft.com/data/equities/tearsheet/summary?s=ORA:PAR</t>
   </si>
   <si>
@@ -1756,9 +1735,6 @@
   </si>
   <si>
     <t>Herige</t>
-  </si>
-  <si>
-    <t>https://markets.ft.com/data/equities/tearsheet/summary?s=HERIG:PAR</t>
   </si>
   <si>
     <t>21/20</t>
@@ -5537,8 +5513,8 @@
   <dimension ref="A1:AQ190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C162" sqref="C162"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="36.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5563,19 +5539,19 @@
   <sheetData>
     <row r="1" spans="1:43" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="8" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>203</v>
@@ -5587,22 +5563,22 @@
         <v>204</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="S1" s="8" t="s">
         <v>205</v>
@@ -5611,19 +5587,19 @@
         <v>206</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="Y1" s="9" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="Z1" s="9" t="s">
         <v>207</v>
@@ -5638,15 +5614,15 @@
         <v>119</v>
       </c>
       <c r="AE1" s="57" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>185</v>
@@ -5733,7 +5709,7 @@
         <v>182</v>
       </c>
       <c r="AE2" s="58" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5775,7 +5751,7 @@
       <c r="AB3" s="13"/>
       <c r="AD3" s="50"/>
       <c r="AE3" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="AQ3" s="50"/>
     </row>
@@ -5787,10 +5763,10 @@
         <v>111</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
@@ -5818,7 +5794,7 @@
       <c r="AB4" s="13"/>
       <c r="AD4" s="50"/>
       <c r="AE4" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="AQ4" s="50"/>
     </row>
@@ -5830,10 +5806,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -5861,7 +5837,7 @@
       <c r="AB5" s="13"/>
       <c r="AD5" s="50"/>
       <c r="AE5" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="AQ5" s="50"/>
     </row>
@@ -5870,13 +5846,13 @@
         <v>123</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -5904,7 +5880,7 @@
       <c r="AB6" s="13"/>
       <c r="AD6" s="50"/>
       <c r="AE6" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="AQ6" s="50"/>
     </row>
@@ -5916,10 +5892,10 @@
         <v>50</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -5947,7 +5923,7 @@
       <c r="AB7" s="13"/>
       <c r="AD7" s="50"/>
       <c r="AE7" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="AQ7" s="50"/>
     </row>
@@ -5959,10 +5935,10 @@
         <v>57</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -5990,7 +5966,7 @@
       <c r="AB8" s="13"/>
       <c r="AD8" s="50"/>
       <c r="AE8" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="AQ8" s="50"/>
     </row>
@@ -6041,10 +6017,10 @@
         <v>19</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -6080,9 +6056,7 @@
         <v>90</v>
       </c>
       <c r="C11" s="16"/>
-      <c r="D11" s="14" t="s">
-        <v>256</v>
-      </c>
+      <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="13"/>
@@ -6154,10 +6128,10 @@
         <v>44</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -6193,10 +6167,10 @@
         <v>47</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -6232,10 +6206,10 @@
         <v>89</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -6310,10 +6284,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -6349,10 +6323,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
@@ -6388,10 +6362,10 @@
         <v>112</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
@@ -6427,10 +6401,10 @@
         <v>53</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
@@ -6466,11 +6440,9 @@
         <v>108</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>272</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="13"/>
@@ -6505,10 +6477,10 @@
         <v>105</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
@@ -6544,11 +6516,9 @@
         <v>107</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>274</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="13"/>
@@ -6583,10 +6553,10 @@
         <v>39</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -6622,10 +6592,10 @@
         <v>45</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
@@ -6661,10 +6631,10 @@
         <v>106</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
@@ -6700,10 +6670,10 @@
         <v>48</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
@@ -6739,10 +6709,10 @@
         <v>60</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
@@ -6775,13 +6745,13 @@
         <v>127</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -6814,13 +6784,13 @@
         <v>127</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
@@ -6853,13 +6823,13 @@
         <v>127</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
@@ -6895,10 +6865,10 @@
         <v>18</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
@@ -6934,10 +6904,10 @@
         <v>40</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
@@ -6973,10 +6943,10 @@
         <v>73</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
@@ -7012,10 +6982,10 @@
         <v>54</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
@@ -7051,10 +7021,10 @@
         <v>129</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
@@ -7087,12 +7057,10 @@
         <v>128</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="C37" s="16"/>
-      <c r="D37" s="14" t="s">
-        <v>573</v>
-      </c>
+      <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
       <c r="G37" s="3"/>
@@ -7127,10 +7095,10 @@
         <v>184</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
@@ -7166,10 +7134,10 @@
         <v>51</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -7205,10 +7173,10 @@
         <v>77</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
@@ -7244,10 +7212,10 @@
         <v>76</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
@@ -7283,10 +7251,10 @@
         <v>130</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
@@ -7322,10 +7290,10 @@
         <v>65</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
@@ -7361,10 +7329,10 @@
         <v>132</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
@@ -7400,10 +7368,10 @@
         <v>133</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
@@ -7439,10 +7407,10 @@
         <v>25</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
@@ -7478,10 +7446,10 @@
         <v>134</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
@@ -7517,10 +7485,10 @@
         <v>63</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
@@ -7556,10 +7524,10 @@
         <v>4</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
@@ -7595,10 +7563,10 @@
         <v>121</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
@@ -7634,10 +7602,10 @@
         <v>35</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
@@ -7673,10 +7641,10 @@
         <v>5</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
@@ -7712,10 +7680,10 @@
         <v>137</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E53" s="14"/>
       <c r="F53" s="14"/>
@@ -7751,10 +7719,10 @@
         <v>138</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
@@ -7790,10 +7758,10 @@
         <v>139</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E55" s="14"/>
       <c r="F55" s="14"/>
@@ -7829,10 +7797,10 @@
         <v>49</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
@@ -7868,10 +7836,10 @@
         <v>31</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E57" s="14"/>
       <c r="F57" s="14"/>
@@ -7904,13 +7872,13 @@
         <v>140</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
@@ -7946,10 +7914,10 @@
         <v>141</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -7985,10 +7953,10 @@
         <v>55</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -8024,10 +7992,10 @@
         <v>104</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
@@ -8063,10 +8031,10 @@
         <v>142</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
@@ -8102,10 +8070,10 @@
         <v>102</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
@@ -8141,9 +8109,7 @@
         <v>120</v>
       </c>
       <c r="C64" s="16"/>
-      <c r="D64" s="14" t="s">
-        <v>364</v>
-      </c>
+      <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="14"/>
       <c r="G64" s="3"/>
@@ -8178,10 +8144,10 @@
         <v>22</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E65" s="14"/>
       <c r="F65" s="14"/>
@@ -8217,10 +8183,10 @@
         <v>181</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
@@ -8253,13 +8219,13 @@
         <v>144</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
@@ -8295,10 +8261,10 @@
         <v>145</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
@@ -8334,10 +8300,10 @@
         <v>146</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
@@ -8373,10 +8339,10 @@
         <v>147</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="E70" s="14"/>
       <c r="F70" s="14"/>
@@ -8412,10 +8378,10 @@
         <v>183</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
@@ -8451,10 +8417,10 @@
         <v>149</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E72" s="14"/>
       <c r="F72" s="14"/>
@@ -8490,10 +8456,10 @@
         <v>150</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="E73" s="14"/>
       <c r="F73" s="14"/>
@@ -8529,10 +8495,10 @@
         <v>42</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
@@ -8565,13 +8531,13 @@
         <v>144</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E75" s="14"/>
       <c r="F75" s="14"/>
@@ -8607,10 +8573,10 @@
         <v>148</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E76" s="14"/>
       <c r="F76" s="14"/>
@@ -8646,10 +8612,10 @@
         <v>9</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E77" s="14"/>
       <c r="F77" s="14"/>
@@ -8729,10 +8695,10 @@
         <v>152</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E79" s="14"/>
       <c r="F79" s="14"/>
@@ -8773,10 +8739,10 @@
         <v>11</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E80" s="14"/>
       <c r="F80" s="14"/>
@@ -8861,10 +8827,10 @@
         <v>23</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E82" s="14"/>
       <c r="F82" s="14"/>
@@ -8905,10 +8871,10 @@
         <v>30</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E83" s="14"/>
       <c r="F83" s="14"/>
@@ -8944,10 +8910,10 @@
         <v>37</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="E84" s="14"/>
       <c r="F84" s="14"/>
@@ -8983,10 +8949,10 @@
         <v>66</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="E85" s="14"/>
       <c r="F85" s="14"/>
@@ -9022,10 +8988,10 @@
         <v>41</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="E86" s="14"/>
       <c r="F86" s="14"/>
@@ -9061,10 +9027,10 @@
         <v>52</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E87" s="14"/>
       <c r="F87" s="14"/>
@@ -9100,10 +9066,10 @@
         <v>153</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="E88" s="14"/>
       <c r="F88" s="14"/>
@@ -9139,10 +9105,10 @@
         <v>28</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="E89" s="14"/>
       <c r="F89" s="14"/>
@@ -9178,10 +9144,10 @@
         <v>155</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E90" s="14"/>
       <c r="F90" s="14"/>
@@ -9217,10 +9183,10 @@
         <v>3</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="E91" s="14"/>
       <c r="F91" s="14"/>
@@ -9256,10 +9222,10 @@
         <v>86</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E92" s="14"/>
       <c r="F92" s="14"/>
@@ -9295,10 +9261,10 @@
         <v>33</v>
       </c>
       <c r="C93" s="16" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="E93" s="14"/>
       <c r="F93" s="14"/>
@@ -9334,10 +9300,10 @@
         <v>34</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="E94" s="14"/>
       <c r="F94" s="14"/>
@@ -9373,10 +9339,10 @@
         <v>36</v>
       </c>
       <c r="C95" s="16" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E95" s="14"/>
       <c r="F95" s="14"/>
@@ -9412,10 +9378,10 @@
         <v>157</v>
       </c>
       <c r="C96" s="16" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E96" s="14"/>
       <c r="F96" s="14"/>
@@ -9451,10 +9417,10 @@
         <v>46</v>
       </c>
       <c r="C97" s="16" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="E97" s="14"/>
       <c r="F97" s="14"/>
@@ -9490,10 +9456,10 @@
         <v>158</v>
       </c>
       <c r="C98" s="16" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="E98" s="14"/>
       <c r="F98" s="14"/>
@@ -9529,10 +9495,10 @@
         <v>56</v>
       </c>
       <c r="C99" s="16" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="E99" s="14"/>
       <c r="F99" s="14"/>
@@ -9568,10 +9534,10 @@
         <v>59</v>
       </c>
       <c r="C100" s="16" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="E100" s="14"/>
       <c r="F100" s="14"/>
@@ -9607,10 +9573,10 @@
         <v>62</v>
       </c>
       <c r="C101" s="16" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="E101" s="14"/>
       <c r="F101" s="14"/>
@@ -9646,9 +9612,7 @@
         <v>161</v>
       </c>
       <c r="C102" s="16"/>
-      <c r="D102" s="14" t="s">
-        <v>433</v>
-      </c>
+      <c r="D102" s="14"/>
       <c r="E102" s="14"/>
       <c r="F102" s="14"/>
       <c r="G102" s="3"/>
@@ -9683,10 +9647,10 @@
         <v>162</v>
       </c>
       <c r="C103" s="16" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="E103" s="14"/>
       <c r="F103" s="14"/>
@@ -9722,10 +9686,10 @@
         <v>101</v>
       </c>
       <c r="C104" s="16" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="E104" s="14"/>
       <c r="F104" s="14"/>
@@ -9761,10 +9725,10 @@
         <v>160</v>
       </c>
       <c r="C105" s="16" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="E105" s="14"/>
       <c r="F105" s="14"/>
@@ -9800,10 +9764,10 @@
         <v>38</v>
       </c>
       <c r="C106" s="16" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="E106" s="14"/>
       <c r="F106" s="14"/>
@@ -9839,10 +9803,10 @@
         <v>58</v>
       </c>
       <c r="C107" s="16" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="E107" s="14"/>
       <c r="F107" s="14"/>
@@ -10073,10 +10037,10 @@
         <v>167</v>
       </c>
       <c r="C113" s="16" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="E113" s="14"/>
       <c r="F113" s="14"/>
@@ -10112,10 +10076,10 @@
         <v>93</v>
       </c>
       <c r="C114" s="16" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E114" s="14"/>
       <c r="F114" s="14"/>
@@ -10151,10 +10115,10 @@
         <v>24</v>
       </c>
       <c r="C115" s="16" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="E115" s="14"/>
       <c r="F115" s="14"/>
@@ -10190,10 +10154,10 @@
         <v>26</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E116" s="14"/>
       <c r="F116" s="14"/>
@@ -10229,10 +10193,10 @@
         <v>168</v>
       </c>
       <c r="C117" s="16" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="E117" s="14"/>
       <c r="F117" s="14"/>
@@ -10268,10 +10232,10 @@
         <v>98</v>
       </c>
       <c r="C118" s="16" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="E118" s="14"/>
       <c r="F118" s="14"/>
@@ -10307,10 +10271,10 @@
         <v>169</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E119" s="14"/>
       <c r="F119" s="14"/>
@@ -10346,10 +10310,10 @@
         <v>32</v>
       </c>
       <c r="C120" s="16" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="D120" s="14" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="E120" s="14"/>
       <c r="F120" s="14"/>
@@ -10385,10 +10349,10 @@
         <v>70</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="E121" s="14"/>
       <c r="F121" s="14"/>
@@ -10424,10 +10388,10 @@
         <v>71</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="E122" s="14"/>
       <c r="F122" s="14"/>
@@ -10463,10 +10427,10 @@
         <v>170</v>
       </c>
       <c r="C123" s="16" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="E123" s="14"/>
       <c r="F123" s="14"/>
@@ -10502,10 +10466,10 @@
         <v>92</v>
       </c>
       <c r="C124" s="16" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="E124" s="14"/>
       <c r="F124" s="14"/>
@@ -10541,10 +10505,10 @@
         <v>43</v>
       </c>
       <c r="C125" s="16" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="E125" s="14"/>
       <c r="F125" s="14"/>
@@ -10580,10 +10544,10 @@
         <v>91</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D126" s="14" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="E126" s="14"/>
       <c r="F126" s="14"/>
@@ -10619,10 +10583,10 @@
         <v>171</v>
       </c>
       <c r="C127" s="16" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="D127" s="14" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="E127" s="14"/>
       <c r="F127" s="14"/>
@@ -10658,10 +10622,10 @@
         <v>97</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="E128" s="14"/>
       <c r="F128" s="14"/>
@@ -10697,10 +10661,10 @@
         <v>95</v>
       </c>
       <c r="C129" s="16" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D129" s="14" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="E129" s="14"/>
       <c r="F129" s="14"/>
@@ -10775,10 +10739,10 @@
         <v>75</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="E131" s="14"/>
       <c r="F131" s="14"/>
@@ -10814,10 +10778,10 @@
         <v>83</v>
       </c>
       <c r="C132" s="16" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="D132" s="14" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="E132" s="14"/>
       <c r="F132" s="14"/>
@@ -10853,10 +10817,10 @@
         <v>0</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="E133" s="14"/>
       <c r="F133" s="14"/>
@@ -10892,10 +10856,10 @@
         <v>21</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="D134" s="14" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="E134" s="14"/>
       <c r="F134" s="14"/>
@@ -10931,10 +10895,10 @@
         <v>74</v>
       </c>
       <c r="C135" s="16" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="D135" s="14" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="E135" s="14"/>
       <c r="F135" s="14"/>
@@ -10970,10 +10934,10 @@
         <v>116</v>
       </c>
       <c r="C136" s="16" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="E136" s="14"/>
       <c r="F136" s="14"/>
@@ -11009,10 +10973,10 @@
         <v>68</v>
       </c>
       <c r="C137" s="16" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="D137" s="14" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="E137" s="14"/>
       <c r="F137" s="14"/>
@@ -11048,10 +11012,10 @@
         <v>173</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="D138" s="14" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="E138" s="14"/>
       <c r="F138" s="14"/>
@@ -11087,10 +11051,10 @@
         <v>115</v>
       </c>
       <c r="C139" s="16" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="E139" s="14"/>
       <c r="F139" s="14"/>
@@ -11126,10 +11090,10 @@
         <v>84</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="E140" s="14"/>
       <c r="F140" s="14"/>
@@ -11165,10 +11129,10 @@
         <v>109</v>
       </c>
       <c r="C141" s="16" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D141" s="14" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="E141" s="14"/>
       <c r="F141" s="14"/>
@@ -11204,10 +11168,10 @@
         <v>110</v>
       </c>
       <c r="C142" s="16" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="D142" s="14" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="E142" s="14"/>
       <c r="F142" s="14"/>
@@ -11243,10 +11207,10 @@
         <v>174</v>
       </c>
       <c r="C143" s="16" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="E143" s="14"/>
       <c r="F143" s="14"/>
@@ -11282,10 +11246,10 @@
         <v>113</v>
       </c>
       <c r="C144" s="16" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="E144" s="14"/>
       <c r="F144" s="14"/>
@@ -11321,10 +11285,10 @@
         <v>114</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="E145" s="14"/>
       <c r="F145" s="14"/>
@@ -11360,10 +11324,10 @@
         <v>175</v>
       </c>
       <c r="C146" s="16" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="E146" s="14"/>
       <c r="F146" s="14"/>
@@ -11399,10 +11363,10 @@
         <v>176</v>
       </c>
       <c r="C147" s="16" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="E147" s="14"/>
       <c r="F147" s="14"/>
@@ -11438,10 +11402,10 @@
         <v>100</v>
       </c>
       <c r="C148" s="16" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="D148" s="14" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="E148" s="14"/>
       <c r="F148" s="14"/>
@@ -11477,10 +11441,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="16" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="D149" s="14" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="E149" s="14"/>
       <c r="F149" s="14"/>
@@ -11516,10 +11480,10 @@
         <v>67</v>
       </c>
       <c r="C150" s="16" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="D150" s="14" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="E150" s="14"/>
       <c r="F150" s="14"/>
@@ -11555,10 +11519,10 @@
         <v>99</v>
       </c>
       <c r="C151" s="16" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="E151" s="14"/>
       <c r="F151" s="14"/>
@@ -11633,9 +11597,7 @@
         <v>79</v>
       </c>
       <c r="C153" s="16"/>
-      <c r="D153" s="14" t="s">
-        <v>236</v>
-      </c>
+      <c r="D153" s="14"/>
       <c r="E153" s="14"/>
       <c r="F153" s="14"/>
       <c r="G153" s="3"/>
@@ -11670,10 +11632,10 @@
         <v>13</v>
       </c>
       <c r="C154" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="D154" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="D154" s="14" t="s">
-        <v>238</v>
       </c>
       <c r="E154" s="14"/>
       <c r="F154" s="14"/>
@@ -11709,10 +11671,10 @@
         <v>80</v>
       </c>
       <c r="C155" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="D155" s="14" t="s">
         <v>239</v>
-      </c>
-      <c r="D155" s="14" t="s">
-        <v>240</v>
       </c>
       <c r="E155" s="14"/>
       <c r="F155" s="14"/>
@@ -11748,10 +11710,10 @@
         <v>16</v>
       </c>
       <c r="C156" s="16" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="D156" s="14" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="E156" s="14"/>
       <c r="F156" s="14"/>
@@ -11787,10 +11749,10 @@
         <v>87</v>
       </c>
       <c r="C157" s="16" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="E157" s="14"/>
       <c r="F157" s="14"/>
@@ -11826,10 +11788,10 @@
         <v>20</v>
       </c>
       <c r="C158" s="16" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E158" s="14"/>
       <c r="F158" s="14"/>
@@ -11865,10 +11827,10 @@
         <v>88</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="E159" s="14"/>
       <c r="F159" s="14"/>
@@ -11904,10 +11866,10 @@
         <v>78</v>
       </c>
       <c r="C160" s="16" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="E160" s="14"/>
       <c r="F160" s="14"/>
@@ -11943,10 +11905,10 @@
         <v>81</v>
       </c>
       <c r="C161" s="16" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="E161" s="14"/>
       <c r="F161" s="14"/>
@@ -11979,12 +11941,10 @@
         <v>177</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="C162" s="16"/>
-      <c r="D162" s="14" t="s">
-        <v>536</v>
-      </c>
+      <c r="D162" s="14"/>
       <c r="E162" s="14"/>
       <c r="F162" s="14"/>
       <c r="G162" s="13"/>
@@ -12019,10 +11979,10 @@
         <v>27</v>
       </c>
       <c r="C163" s="16" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="E163" s="14"/>
       <c r="F163" s="14"/>
@@ -12058,10 +12018,10 @@
         <v>29</v>
       </c>
       <c r="C164" s="16" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="E164" s="14"/>
       <c r="F164" s="14"/>
@@ -12097,10 +12057,10 @@
         <v>178</v>
       </c>
       <c r="C165" s="16" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="E165" s="14"/>
       <c r="F165" s="14"/>
@@ -12136,10 +12096,10 @@
         <v>122</v>
       </c>
       <c r="C166" s="16" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="D166" s="14" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="E166" s="14"/>
       <c r="F166" s="14"/>
@@ -12175,10 +12135,10 @@
         <v>6</v>
       </c>
       <c r="C167" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="D167" s="14" t="s">
         <v>241</v>
-      </c>
-      <c r="D167" s="14" t="s">
-        <v>242</v>
       </c>
       <c r="E167" s="14"/>
       <c r="F167" s="14"/>
@@ -12214,10 +12174,10 @@
         <v>7</v>
       </c>
       <c r="C168" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="D168" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="D168" s="14" t="s">
-        <v>244</v>
       </c>
       <c r="E168" s="14"/>
       <c r="F168" s="14"/>
@@ -12253,10 +12213,10 @@
         <v>8</v>
       </c>
       <c r="C169" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D169" s="14" t="s">
         <v>245</v>
-      </c>
-      <c r="D169" s="14" t="s">
-        <v>246</v>
       </c>
       <c r="E169" s="14"/>
       <c r="F169" s="14"/>
@@ -12292,10 +12252,10 @@
         <v>180</v>
       </c>
       <c r="C170" s="16" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="D170" s="14" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="E170" s="14"/>
       <c r="F170" s="14"/>
@@ -12331,10 +12291,10 @@
         <v>118</v>
       </c>
       <c r="C171" s="16" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="D171" s="14" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="E171" s="14"/>
       <c r="F171" s="14"/>
@@ -12367,13 +12327,13 @@
         <v>179</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="C172" s="16" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="E172" s="14"/>
       <c r="F172" s="14"/>
@@ -12409,10 +12369,10 @@
         <v>117</v>
       </c>
       <c r="C173" s="16" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="D173" s="14" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="E173" s="14"/>
       <c r="F173" s="14"/>
@@ -12581,120 +12541,117 @@
     <hyperlink ref="D7" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
     <hyperlink ref="D8" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="D10" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="D11" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="D15" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="D17" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="D19" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="D28" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C23" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C21" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C27" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C26" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C24" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C22" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="C28" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="C25" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C13" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C15" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="C10" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="C8" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="C7" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="C4" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="C169" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="C167" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="D169" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="D168" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D167" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="C152" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="D152" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="D153" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D154" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="D155" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="C130" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D130" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="D81" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="C3" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="D3" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="C9" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="C16" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="C92" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="C140" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="D140" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="C145" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="D157" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="C158" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="D158" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="C78" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="D78" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="D128" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="C128" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="C119" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="D119" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="D112" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="C112" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="D111" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="C111" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D110" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="C110" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="C109" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="D109" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="D108" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="C108" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="C114" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="C14" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="C17" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C85" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="C31" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="C30" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="C39" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="C103" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="C107" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="C97" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="C68" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="C104" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D104" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="D67" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="C67" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="D70" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="D172" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="C172" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="D162" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="C105" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="C117" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="C118" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="C61" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="C60" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="D62" r:id="rId121" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="C62" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="C58" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="C5" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="C6" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="D6" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="C29" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="D29" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="C157" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="C173" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="D30" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="C19" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="C44" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="C147" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="AE2" r:id="rId135" location="Benefice-net-par-action-BNA-282" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="C122" r:id="rId136" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="C123" r:id="rId137" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="C159" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="C133" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="C75" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="D15" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="D17" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="D19" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D28" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C23" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C21" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C27" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C26" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C24" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C22" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C28" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C25" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C13" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C15" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C10" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C8" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C7" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C4" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C169" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C167" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="D169" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="D168" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D167" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C152" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="D152" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="D154" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="D155" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C130" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D130" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D81" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="C3" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="D3" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="C9" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="C16" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="C92" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C140" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="D140" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="C145" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="D157" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="C158" r:id="rId77" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="D158" r:id="rId78" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="C78" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="D78" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="D128" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="C128" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="C119" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="D119" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="D112" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="C112" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="D111" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="C111" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="D110" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="C110" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="C109" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="D109" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="D108" r:id="rId93" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="C108" r:id="rId94" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="C114" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="C14" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="C17" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C85" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="C31" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="C30" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="C39" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="C103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="C107" r:id="rId103" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="C97" r:id="rId104" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="C68" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="C104" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="D104" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="D67" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="C67" r:id="rId109" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="D70" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="D172" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="C172" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="C105" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="C117" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="C118" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="C61" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="C60" r:id="rId117" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="D62" r:id="rId118" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="C62" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="C58" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="C5" r:id="rId121" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="C6" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="D6" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="C29" r:id="rId124" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="D29" r:id="rId125" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="C157" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="C173" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="D30" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="C19" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="C44" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="C147" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="AE2" r:id="rId132" location="Benefice-net-par-action-BNA-282" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="C122" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="C123" r:id="rId134" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="C159" r:id="rId135" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="C133" r:id="rId136" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="C75" r:id="rId137" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId141"/>
-  <drawing r:id="rId142"/>
-  <legacyDrawing r:id="rId143"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId138"/>
+  <drawing r:id="rId139"/>
+  <legacyDrawing r:id="rId140"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId144" name="Bouton 1">
+            <control shapeId="1025" r:id="rId141" name="Bouton 1">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!lancement_scraping">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -12756,90 +12713,90 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="I1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="J1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="K1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="L1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="M1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="N1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="O1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="P1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="Q1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="R1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="S1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="T1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="U1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="V1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="W1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="X1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="Y1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="Z1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="AA1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="AB1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C2" s="39">
         <v>16</v>
@@ -12860,7 +12817,7 @@
         <v>21</v>
       </c>
       <c r="I2" s="40" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="J2" s="39">
         <v>15</v>
@@ -12884,7 +12841,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="40" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="R2" s="39">
         <v>16</v>
@@ -12905,26 +12862,26 @@
         <v>21</v>
       </c>
       <c r="X2" s="40" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y2" s="40" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="Z2" s="40" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="AA2" s="40" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="AB2" s="40" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="AC2" s="39" t="str">
         <f>Actions!AC2</f>
         <v>Beta</v>
       </c>
       <c r="AD2" s="41" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13275,7 +13232,7 @@
         <v>Aéronautique - défense</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="C6" s="44"/>
       <c r="D6" s="44">
@@ -39138,7 +39095,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>217</v>
@@ -39149,7 +39106,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>218</v>
@@ -39160,7 +39117,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>219</v>
@@ -39215,7 +39172,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>217</v>
@@ -39226,7 +39183,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>218</v>
@@ -39237,7 +39194,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>219</v>
@@ -39248,7 +39205,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>221</v>
@@ -39264,7 +39221,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>